<commit_message>
feat: columnas finales (TOTAL CARGA, IVA, SIN IVA) en script y web
</commit_message>
<xml_diff>
--- a/boletas.xlsx
+++ b/boletas.xlsx
@@ -471,17 +471,17 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Importe diferencia</t>
+          <t>TOTAL CARGA</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Diferencia (antes - acreditar)</t>
+          <t>IVA</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Resta: Importe diferencia - Diferencia (antes - acreditar)</t>
+          <t>SIN IVA</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(IVA): SIN IVA=TOTAL/1.21; IVA=TOTAL-SINIVA en web y script; regen
</commit_message>
<xml_diff>
--- a/boletas.xlsx
+++ b/boletas.xlsx
@@ -528,12 +528,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>202109,28</t>
+          <t>950583,84</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>5275064,27</t>
+          <t>4526589,71</t>
         </is>
       </c>
     </row>
@@ -580,12 +580,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>451263,69</t>
+          <t>2136683,58</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>11860103,63</t>
+          <t>10174683,74</t>
         </is>
       </c>
     </row>
@@ -632,12 +632,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>499314,65</t>
+          <t>2352355,34</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>13054732,78</t>
+          <t>11201692,09</t>
         </is>
       </c>
     </row>
@@ -684,12 +684,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>579279,91</t>
+          <t>2706498,40</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>15015306,12</t>
+          <t>12888087,63</t>
         </is>
       </c>
     </row>
@@ -736,12 +736,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>138602,48</t>
+          <t>648648,75</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>3598849,84</t>
+          <t>3088803,57</t>
         </is>
       </c>
     </row>
@@ -788,12 +788,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>130733,60</t>
+          <t>613858,47</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>3406260,42</t>
+          <t>2923135,55</t>
         </is>
       </c>
     </row>
@@ -840,12 +840,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>135633,12</t>
+          <t>597231,09</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>3305555,56</t>
+          <t>2843957,59</t>
         </is>
       </c>
     </row>
@@ -892,12 +892,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>135694,17</t>
+          <t>558603,21</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>3082924,31</t>
+          <t>2660015,27</t>
         </is>
       </c>
     </row>
@@ -944,12 +944,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>332815,19</t>
+          <t>1378033,43</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>7607282,18</t>
+          <t>6562063,94</t>
         </is>
       </c>
     </row>
@@ -996,12 +996,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>129315,81</t>
+          <t>531578,91</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>2933591,23</t>
+          <t>2531328,13</t>
         </is>
       </c>
     </row>
@@ -1048,12 +1048,12 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>208566,12</t>
+          <t>859830,97</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>4745698,02</t>
+          <t>4094433,17</t>
         </is>
       </c>
     </row>
@@ -1100,12 +1100,12 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>107259,25</t>
+          <t>444756,65</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>2455386,22</t>
+          <t>2117888,82</t>
         </is>
       </c>
     </row>
@@ -1152,12 +1152,12 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>208566,12</t>
+          <t>859830,97</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>4745698,02</t>
+          <t>4094433,17</t>
         </is>
       </c>
     </row>
@@ -1204,12 +1204,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>88874,24</t>
+          <t>344783,12</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1897733,26</t>
+          <t>1641824,38</t>
         </is>
       </c>
     </row>
@@ -1256,12 +1256,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>366067,18</t>
+          <t>1403071,16</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>7718295,22</t>
+          <t>6681291,24</t>
         </is>
       </c>
     </row>
@@ -1308,12 +1308,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>571076,12</t>
+          <t>2197635,14</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>12091488,25</t>
+          <t>10464929,23</t>
         </is>
       </c>
     </row>
@@ -1360,12 +1360,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>331362,80</t>
+          <t>1271752,86</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>6996356,06</t>
+          <t>6055966,00</t>
         </is>
       </c>
     </row>
@@ -1412,12 +1412,12 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>331362,80</t>
+          <t>1271752,86</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>6996356,06</t>
+          <t>6055966,00</t>
         </is>
       </c>
     </row>
@@ -1464,12 +1464,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>258752,11</t>
+          <t>989111,56</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>5440414,51</t>
+          <t>4710055,06</t>
         </is>
       </c>
     </row>
@@ -1516,12 +1516,12 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>214752,42</t>
+          <t>945615,89</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>5233796,30</t>
+          <t>4502932,83</t>
         </is>
       </c>
     </row>
@@ -1568,12 +1568,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>188379,33</t>
+          <t>829487,63</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>4591049,38</t>
+          <t>3949941,08</t>
         </is>
       </c>
     </row>
@@ -1620,12 +1620,12 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>118293,00</t>
+          <t>488378,47</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>2695697,25</t>
+          <t>2325611,78</t>
         </is>
       </c>
     </row>
@@ -1672,12 +1672,12 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>309593,32</t>
+          <t>1189793,09</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>6545881,13</t>
+          <t>5665681,36</t>
         </is>
       </c>
     </row>
@@ -1724,12 +1724,12 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>133051,21</t>
+          <t>507928,62</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>2793585,10</t>
+          <t>2418707,69</t>
         </is>
       </c>
     </row>
@@ -1776,12 +1776,12 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>258752,11</t>
+          <t>989111,56</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>5440414,51</t>
+          <t>4710055,06</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(aranceles): columnas ARANCELES CON IVA, IVA ARANCELES, ARANCELES SIN IVA; regen
</commit_message>
<xml_diff>
--- a/boletas.xlsx
+++ b/boletas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,21 @@
           <t>SIN IVA</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>ARANCELES CON IVA</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>IVA ARANCELES</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>ARANCELES SIN IVA</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -536,6 +551,21 @@
           <t>4526589,71</t>
         </is>
       </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>202109,28</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>167032,46</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>35076,82</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -588,6 +618,21 @@
           <t>10174683,74</t>
         </is>
       </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>451263,69</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>372945,20</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>78318,49</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -640,6 +685,21 @@
           <t>11201692,09</t>
         </is>
       </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>499314,65</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>412656,74</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>86657,91</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -692,6 +752,21 @@
           <t>12888087,63</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>579279,91</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>478743,73</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>100536,18</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -744,6 +819,21 @@
           <t>3088803,57</t>
         </is>
       </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>138602,48</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>114547,50</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>24054,98</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -796,6 +886,21 @@
           <t>2923135,55</t>
         </is>
       </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>130733,60</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>108044,30</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>22689,30</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -848,6 +953,21 @@
           <t>2843957,59</t>
         </is>
       </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>135633,12</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>112093,49</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>23539,63</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -900,6 +1020,21 @@
           <t>2660015,27</t>
         </is>
       </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>135694,17</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>112143,94</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>23550,23</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -952,6 +1087,21 @@
           <t>6562063,94</t>
         </is>
       </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>332815,19</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>275053,88</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>57761,31</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1004,6 +1154,21 @@
           <t>2531328,13</t>
         </is>
       </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>129315,81</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>106872,57</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>22443,24</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1056,6 +1221,21 @@
           <t>4094433,17</t>
         </is>
       </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>208566,12</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>172368,69</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>36197,43</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1108,6 +1288,21 @@
           <t>2117888,82</t>
         </is>
       </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>107259,25</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>88644,01</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>18615,24</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1160,6 +1355,21 @@
           <t>4094433,17</t>
         </is>
       </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>208566,12</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>172368,69</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>36197,43</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1212,6 +1422,21 @@
           <t>1641824,38</t>
         </is>
       </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>88874,24</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>73449,79</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>15424,45</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1264,6 +1489,21 @@
           <t>6681291,24</t>
         </is>
       </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>366067,18</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>302534,86</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>63532,32</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1316,6 +1556,21 @@
           <t>10464929,23</t>
         </is>
       </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>571076,12</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>471963,74</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>99112,38</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1368,6 +1623,21 @@
           <t>6055966,00</t>
         </is>
       </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>331362,80</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>273853,55</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>57509,25</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1420,6 +1690,21 @@
           <t>6055966,00</t>
         </is>
       </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>331362,80</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>273853,55</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>57509,25</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1472,6 +1757,21 @@
           <t>4710055,06</t>
         </is>
       </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>258752,11</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>213844,72</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>44907,39</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1524,6 +1824,21 @@
           <t>4502932,83</t>
         </is>
       </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>214752,42</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>177481,34</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>37271,08</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1576,6 +1891,21 @@
           <t>3949941,08</t>
         </is>
       </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>188379,33</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>155685,40</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>32693,93</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1628,6 +1958,21 @@
           <t>2325611,78</t>
         </is>
       </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>118293,00</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>97762,81</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>20530,19</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1680,6 +2025,21 @@
           <t>5665681,36</t>
         </is>
       </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>309593,32</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>255862,25</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>53731,07</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1732,6 +2092,21 @@
           <t>2418707,69</t>
         </is>
       </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>133051,21</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>109959,68</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>23091,53</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1782,6 +2157,21 @@
       <c r="J26" t="inlineStr">
         <is>
           <t>4710055,06</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>258752,11</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>213844,72</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>44907,39</t>
         </is>
       </c>
     </row>

</xml_diff>